<commit_message>
changed algorithm to select best sparse matrix
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_Definition.xlsx
+++ b/NewCDSDataFromClient/CDS_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_main\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CA7444-8E29-410A-8F00-072DD0FC75C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07E12CD-E5E6-42A8-832F-9BE15E5C8FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition_General" sheetId="1" r:id="rId1"/>
@@ -739,7 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4990CF-594D-44E7-8ED2-EB98FC4D9840}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>